<commit_message>
updated audit code for modify & suspended
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/ServiceRoleMapping_BBA9WithJSR.xlsx
+++ b/src/integrationTest/resources/ServiceRoleMapping_BBA9WithJSR.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/350950/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BA49DF-DAC3-3842-8436-CEF957930759}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2AE077-A240-D24D-9268-8F4B870827FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="14500" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
   </bookViews>
   <sheets>
-    <sheet name="IDAM Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="Service to CW Roles Mapping" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -415,7 +415,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>